<commit_message>
updated first part by Hieu
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75246088-7F42-4F66-9ADB-0F552ACF1403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094C615-51E2-448E-B42E-C7073F642468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -135,7 +135,10 @@
     <t>30/04</t>
   </si>
   <si>
-    <t>Hieu</t>
+    <t>Trí</t>
+  </si>
+  <si>
+    <t>Hiếu</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:J992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -723,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -880,10 +883,10 @@
         <v>45662</v>
       </c>
       <c r="D8" s="9">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -905,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -927,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -949,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -961,10 +964,18 @@
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="8">
+        <v>45693</v>
+      </c>
+      <c r="C12" s="8">
+        <v>45693</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="11"/>
@@ -975,10 +986,18 @@
       <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="21"/>
+      <c r="B13" s="8">
+        <v>45693</v>
+      </c>
+      <c r="C13" s="8">
+        <v>45693</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>32</v>
+      </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="11"/>
@@ -992,7 +1011,9 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="21"/>
+      <c r="E14" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="11"/>
@@ -1006,7 +1027,9 @@
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="11"/>
@@ -1020,7 +1043,9 @@
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="21"/>
+      <c r="E16" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="11"/>
@@ -1034,7 +1059,9 @@
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="21"/>
+      <c r="E17" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="11"/>
@@ -1048,7 +1075,9 @@
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="21"/>
+      <c r="E18" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
@@ -1062,7 +1091,9 @@
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="21"/>
+      <c r="E19" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="11"/>
@@ -1076,7 +1107,9 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="11"/>

</xml_diff>